<commit_message>
Changes to Student Upload
</commit_message>
<xml_diff>
--- a/Sample Docs/Students.xlsx
+++ b/Sample Docs/Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vamsi\Desktop\GIT\Resonance\Sample Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05103FAC-8733-4626-B949-08FDB8B2754E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C42D7F-DA82-42E1-BC01-D386E250176B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,12 +81,6 @@
     <t>ProfilePicture</t>
   </si>
   <si>
-    <t>RC2</t>
-  </si>
-  <si>
-    <t>xxx</t>
-  </si>
-  <si>
     <t>yyy</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>fdgfd</t>
   </si>
   <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
     <t>Telangana</t>
   </si>
   <si>
@@ -115,6 +106,15 @@
   </si>
   <si>
     <t>Class 12/NEET</t>
+  </si>
+  <si>
+    <t>RC3</t>
+  </si>
+  <si>
+    <t>Mehboobnagar</t>
+  </si>
+  <si>
+    <t>Ramya</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,46 +553,46 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
         <v>44567</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="1">
         <v>38364</v>
       </c>
       <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
       </c>
       <c r="L2">
         <v>345678</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O2">
         <v>9999999999</v>
@@ -601,7 +601,7 @@
         <v>754567</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DB Design for Chapters
</commit_message>
<xml_diff>
--- a/Sample Docs/Students.xlsx
+++ b/Sample Docs/Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vamsi\Desktop\GIT\Resonance\Sample Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C42D7F-DA82-42E1-BC01-D386E250176B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE5A9A1-27F5-4254-87A1-761A4ABB2600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>AdmissionId</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>RC3</t>
-  </si>
-  <si>
-    <t>Mehboobnagar</t>
   </si>
   <si>
     <t>Ramya</t>
@@ -471,7 +468,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +556,7 @@
         <v>44567</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -578,9 +575,6 @@
       </c>
       <c r="I2" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
       </c>
       <c r="K2" t="s">
         <v>23</v>

</xml_diff>